<commit_message>
Agrego resultados en xlsx + fechas de tendencias + settings
</commit_message>
<xml_diff>
--- a/Pruebas/historia con calculo RSI y Bandas bollinger - Corregido.xlsx
+++ b/Pruebas/historia con calculo RSI y Bandas bollinger - Corregido.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUSTENTATOR SA\Desktop\Proyectos\Backtesting-crypto-trading\Superados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUSTENTATOR SA\Desktop\Proyectos\Backtesting-crypto-trading\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6866C33E-FCBD-473B-96E8-1CB54FAA2B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D817F-8975-41E2-AB6A-6A1F81118EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="historia" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -112,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -261,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +453,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,7 +635,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -620,19 +647,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="16" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -988,12 +1025,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,6 +1124,7 @@
       <c r="M2" t="s">
         <v>15</v>
       </c>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1116,6 +1154,9 @@
       <c r="M3" t="s">
         <v>15</v>
       </c>
+      <c r="N3" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1145,6 +1186,9 @@
       <c r="M4" t="s">
         <v>15</v>
       </c>
+      <c r="N4" s="6">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1174,6 +1218,9 @@
       <c r="M5" t="s">
         <v>15</v>
       </c>
+      <c r="N5" s="6">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -1203,6 +1250,9 @@
       <c r="M6" t="s">
         <v>15</v>
       </c>
+      <c r="N6" s="6">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1232,6 +1282,9 @@
       <c r="M7" t="s">
         <v>15</v>
       </c>
+      <c r="N7" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1261,6 +1314,9 @@
       <c r="M8" t="s">
         <v>15</v>
       </c>
+      <c r="N8" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1290,6 +1346,9 @@
       <c r="M9" t="s">
         <v>15</v>
       </c>
+      <c r="N9" s="6">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1319,6 +1378,9 @@
       <c r="M10" t="s">
         <v>15</v>
       </c>
+      <c r="N10" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1348,12 +1410,12 @@
       <c r="M11" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1438,7 +1500,7 @@
         <v>10</v>
       </c>
       <c r="O13">
-        <f>E13-E12</f>
+        <f t="shared" ref="O13:O22" si="0">E13-E12</f>
         <v>-3.6000000000058208</v>
       </c>
       <c r="P13" s="6">
@@ -1484,15 +1546,15 @@
         <v>9</v>
       </c>
       <c r="O14">
-        <f>E14-E13</f>
+        <f t="shared" si="0"/>
         <v>-6.7999999999956344</v>
       </c>
       <c r="P14" s="6">
-        <f t="shared" ref="P14:P22" si="0">IF(O14&lt;0,0,ABS(O14))</f>
+        <f t="shared" ref="P14:P22" si="1">IF(O14&lt;0,0,ABS(O14))</f>
         <v>0</v>
       </c>
       <c r="Q14" s="6">
-        <f t="shared" ref="Q14:Q22" si="1">IF(O14&lt;0,ABS(O14),0)</f>
+        <f t="shared" ref="Q14:Q22" si="2">IF(O14&lt;0,ABS(O14),0)</f>
         <v>6.7999999999956344</v>
       </c>
     </row>
@@ -1530,15 +1592,15 @@
         <v>8</v>
       </c>
       <c r="O15">
-        <f>E15-E14</f>
-        <v>7.4000000000014552</v>
-      </c>
-      <c r="P15" s="6">
         <f t="shared" si="0"/>
         <v>7.4000000000014552</v>
       </c>
+      <c r="P15" s="6">
+        <f t="shared" si="1"/>
+        <v>7.4000000000014552</v>
+      </c>
       <c r="Q15" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1578,15 +1640,15 @@
         <v>7</v>
       </c>
       <c r="O16">
-        <f>E16-E15</f>
-        <v>69</v>
-      </c>
-      <c r="P16" s="6">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
+      <c r="P16" s="6">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
       <c r="Q16" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1626,15 +1688,15 @@
         <v>6</v>
       </c>
       <c r="O17">
-        <f>E17-E16</f>
-        <v>53</v>
-      </c>
-      <c r="P17" s="6">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
+      <c r="P17" s="6">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
       <c r="Q17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1674,15 +1736,15 @@
         <v>5</v>
       </c>
       <c r="O18">
-        <f>E18-E17</f>
+        <f t="shared" si="0"/>
         <v>-51.600000000005821</v>
       </c>
       <c r="P18" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51.600000000005821</v>
       </c>
     </row>
@@ -1722,15 +1784,15 @@
         <v>4</v>
       </c>
       <c r="O19">
-        <f>E19-E18</f>
+        <f t="shared" si="0"/>
         <v>-43.5</v>
       </c>
       <c r="P19" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43.5</v>
       </c>
     </row>
@@ -1770,48 +1832,48 @@
         <v>3</v>
       </c>
       <c r="O20">
-        <f>E20-E19</f>
-        <v>19.5</v>
-      </c>
-      <c r="P20" s="6">
         <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
+      <c r="P20" s="6">
+        <f t="shared" si="1"/>
+        <v>19.5</v>
+      </c>
       <c r="Q20" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="9">
         <v>44479.013194444444</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="8">
         <v>54734.7</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="8">
         <v>54763</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="8">
         <v>54728.2</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="8">
         <v>54754.3</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="8">
         <v>62.51</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="8">
         <v>54697.18</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10">
+      <c r="H21" s="8"/>
+      <c r="I21" s="8">
         <v>54690.76</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="8">
         <v>54769.24</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="8">
         <v>54612.27</v>
       </c>
       <c r="L21" t="s">
@@ -1824,15 +1886,15 @@
         <v>2</v>
       </c>
       <c r="O21">
-        <f>E21-E20</f>
-        <v>19.600000000005821</v>
-      </c>
-      <c r="P21" s="6">
         <f t="shared" si="0"/>
         <v>19.600000000005821</v>
       </c>
+      <c r="P21" s="6">
+        <f t="shared" si="1"/>
+        <v>19.600000000005821</v>
+      </c>
       <c r="Q21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1840,32 +1902,32 @@
       <c r="A22" s="3">
         <v>44479.013888888891</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="8">
         <v>54754.3</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="8">
         <v>54754.3</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="8">
         <v>54701</v>
       </c>
       <c r="E22" s="4">
         <v>54717.9</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="11">
         <v>54.28</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="8">
         <v>54704.38</v>
       </c>
       <c r="H22" s="4"/>
-      <c r="I22" s="4">
+      <c r="I22" s="12">
         <v>54693.75</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="14">
         <v>54771.85</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="16">
         <v>54615.64</v>
       </c>
       <c r="L22" t="s">
@@ -1878,15 +1940,15 @@
         <v>1</v>
       </c>
       <c r="O22">
-        <f>E22-E21</f>
+        <f t="shared" si="0"/>
         <v>-36.400000000001455</v>
       </c>
       <c r="P22" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q22" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36.400000000001455</v>
       </c>
       <c r="R22" s="2">
@@ -1975,7 +2037,7 @@
       <c r="M24" t="s">
         <v>15</v>
       </c>
-      <c r="O24" s="8" t="s">
+      <c r="O24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="P24" s="6">
@@ -2021,7 +2083,7 @@
       <c r="M25" t="s">
         <v>15</v>
       </c>
-      <c r="O25" s="8" t="s">
+      <c r="O25" s="7" t="s">
         <v>23</v>
       </c>
       <c r="P25" s="6">
@@ -2067,7 +2129,7 @@
       <c r="M26" t="s">
         <v>15</v>
       </c>
-      <c r="O26" s="8" t="s">
+      <c r="O26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P26" s="6">
@@ -2113,10 +2175,10 @@
       <c r="M27" t="s">
         <v>15</v>
       </c>
-      <c r="O27" s="8" t="s">
+      <c r="O27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P27" s="12">
+      <c r="P27" s="10">
         <f>100-(100/(1+P26))</f>
         <v>54.284793814432533</v>
       </c>
@@ -2159,10 +2221,10 @@
       <c r="M28" t="s">
         <v>15</v>
       </c>
-      <c r="O28" s="8" t="s">
+      <c r="O28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P28" s="9">
+      <c r="P28" s="15">
         <f>R22+1.5*S22</f>
         <v>54771.845115026204</v>
       </c>
@@ -2205,10 +2267,10 @@
       <c r="M29" t="s">
         <v>15</v>
       </c>
-      <c r="O29" s="8" t="s">
+      <c r="O29" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P29" s="9">
+      <c r="P29" s="13">
         <f>R22</f>
         <v>54693.74500000001</v>
       </c>
@@ -2251,10 +2313,10 @@
       <c r="M30" t="s">
         <v>15</v>
       </c>
-      <c r="O30" s="8" t="s">
+      <c r="O30" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P30" s="9">
+      <c r="P30" s="17">
         <f>P29-1.5*S22</f>
         <v>54615.644884973815</v>
       </c>

</xml_diff>